<commit_message>
Add competitive bidding features and UI improvements - New CompetitiveBiddingChat component - Enhanced ERP integration with sales invoice API - Updated workspace navigation and management - Added sample prompts and documentation - Improved property management chat functionality
</commit_message>
<xml_diff>
--- a/public/example_purchase_orders.xlsx
+++ b/public/example_purchase_orders.xlsx
@@ -5,22 +5,38 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikbu\Documents\Retta\vite_app_property_manager_purchaser_assistant\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikbu\Documents\Retta\vite_app_propertius\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED843E2-543C-4B1D-B96B-7694DCF054A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE40E34D-7D60-4867-BA4D-6EABC206EB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{A3B23C0C-A7D8-4F90-8222-F83D4588D6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="property_maintenance_orders.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">property_maintenance_orders.csv!$A$1:$M$35</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="79">
   <si>
     <t>PO Number</t>
   </si>
@@ -76,21 +92,9 @@
     <t>Vendor Order No.</t>
   </si>
   <si>
-    <t>Giro No.</t>
-  </si>
-  <si>
-    <t>VAT Registration No.</t>
-  </si>
-  <si>
-    <t>Shipment Method</t>
-  </si>
-  <si>
     <t>Huolto-Karhu Oy</t>
   </si>
   <si>
-    <t>Huoltotie 12</t>
-  </si>
-  <si>
     <t>FI12345678</t>
   </si>
   <si>
@@ -103,21 +107,12 @@
     <t>Tunti</t>
   </si>
   <si>
-    <t>Mikael JÃ¤rvinen</t>
-  </si>
-  <si>
     <t>040-123-4567</t>
   </si>
   <si>
     <t>mikael@kiinteistopalvelut.fi</t>
   </si>
   <si>
-    <t>888-9999</t>
-  </si>
-  <si>
-    <t>Kuljetus</t>
-  </si>
-  <si>
     <t>KH-202</t>
   </si>
   <si>
@@ -130,9 +125,6 @@
     <t>RakenneFix Oy</t>
   </si>
   <si>
-    <t>Rakennuskatu 5</t>
-  </si>
-  <si>
     <t>FI98765432</t>
   </si>
   <si>
@@ -142,39 +134,24 @@
     <t>Ikkunoiden tiivistys ja korjaus</t>
   </si>
   <si>
-    <t>Erika SundstrÃ¶m</t>
-  </si>
-  <si>
     <t>+46 70 112 3344</t>
   </si>
   <si>
     <t>erika@suomikiinteisto.fi</t>
   </si>
   <si>
-    <t>Nouto</t>
-  </si>
-  <si>
     <t>RF-404</t>
   </si>
   <si>
     <t>Tiivistemassa (silikoni)</t>
   </si>
   <si>
-    <t>KiinteistÃ¶Pro Oy</t>
-  </si>
-  <si>
-    <t>Palvelukatu 3</t>
-  </si>
-  <si>
     <t>FI45678912</t>
   </si>
   <si>
     <t>KP-505</t>
   </si>
   <si>
-    <t>SÃ¤hkÃ¶jÃ¤rjestelmÃ¤n huolto</t>
-  </si>
-  <si>
     <t>Sari Rautakorpi</t>
   </si>
   <si>
@@ -187,18 +164,12 @@
     <t>KP-606</t>
   </si>
   <si>
-    <t>SÃ¤hkÃ¶kaapelit ja liittimet</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
     <t>RakennusMestarit Oy</t>
   </si>
   <si>
-    <t>TyÃ¶tie 8</t>
-  </si>
-  <si>
     <t>FI32165487</t>
   </si>
   <si>
@@ -211,12 +182,6 @@
     <t>RM-808</t>
   </si>
   <si>
-    <t>Maali (sisÃ¤seinÃ¤maali</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10L)</t>
-  </si>
-  <si>
     <t>RM-909</t>
   </si>
   <si>
@@ -238,15 +203,9 @@
     <t>KP-707</t>
   </si>
   <si>
-    <t>LumityÃ¶t ja hiekoitus</t>
-  </si>
-  <si>
     <t>KP-808</t>
   </si>
   <si>
-    <t>Hiekoitussepeli (25kg sÃ¤kki)</t>
-  </si>
-  <si>
     <t>RF-909</t>
   </si>
   <si>
@@ -256,12 +215,6 @@
     <t>RF-101</t>
   </si>
   <si>
-    <t>Lakka (parkettilakka</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5L)</t>
-  </si>
-  <si>
     <t>RM-110</t>
   </si>
   <si>
@@ -274,7 +227,52 @@
     <t>Lukko (Abloy-lukko)</t>
   </si>
   <si>
-    <t>Supplier Address steet address</t>
+    <t>Erika Sundstrom</t>
+  </si>
+  <si>
+    <t>KiinteistoPro Oy</t>
+  </si>
+  <si>
+    <t>Lumityot ja hiekoitus</t>
+  </si>
+  <si>
+    <t>Mikael Jorvinen</t>
+  </si>
+  <si>
+    <t>Sohkojorjestelmon huolto</t>
+  </si>
+  <si>
+    <t>Sohkokaapelit ja liittimet</t>
+  </si>
+  <si>
+    <t>Hiekoitussepeli (25kg sokki)</t>
+  </si>
+  <si>
+    <t>Maali (sisoseinomaali 10 L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakka (parkettilakka 5L) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier Address </t>
+  </si>
+  <si>
+    <t>Huoltotie 12, Vantaa</t>
+  </si>
+  <si>
+    <t>Rakennuskatu 5, Espoo</t>
+  </si>
+  <si>
+    <t>Palvelukatu 3, Helsinki</t>
+  </si>
+  <si>
+    <t>Tyotie 8, Tampere,  Tampere</t>
+  </si>
+  <si>
+    <t>Tyotie 8, Tampere</t>
+  </si>
+  <si>
+    <t>Kattoremontti (peltikaton nosturiavusteinen korjaus)</t>
   </si>
 </sst>
 </file>
@@ -760,12 +758,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1141,92 +1141,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88DF940-443D-4976-9946-15F047AF1151}">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.84375" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="18.84375" customWidth="1"/>
+    <col min="3" max="3" width="26.3828125" customWidth="1"/>
+    <col min="4" max="4" width="34.53515625" customWidth="1"/>
     <col min="5" max="5" width="15.15234375" customWidth="1"/>
     <col min="7" max="7" width="29.53515625" customWidth="1"/>
-    <col min="12" max="12" width="25.3828125" customWidth="1"/>
-    <col min="21" max="21" width="26.07421875" customWidth="1"/>
+    <col min="10" max="10" width="9.23046875" style="4"/>
+    <col min="12" max="12" width="25.3828125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="28.3046875" customWidth="1"/>
+    <col min="16" max="16" width="19.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>107000</v>
       </c>
@@ -1234,45 +1227,46 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
       </c>
       <c r="H2">
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="1">
-        <v>3.5763888888888888</v>
+        <v>22</v>
+      </c>
+      <c r="J2" s="4">
+        <v>70</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="1">
-        <v>35.625</v>
+      <c r="L2" s="4">
+        <f>H2*J2</f>
+        <v>700</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="2">
+        <v>24</v>
+      </c>
+      <c r="P2" s="1">
         <v>45757</v>
       </c>
       <c r="Q2" t="b">
@@ -1284,17 +1278,8 @@
       <c r="S2">
         <v>2001</v>
       </c>
-      <c r="T2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U2">
-        <v>777777777</v>
-      </c>
-      <c r="V2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>107000</v>
       </c>
@@ -1302,45 +1287,46 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.9375</v>
+        <v>27</v>
+      </c>
+      <c r="J3" s="4">
+        <v>94</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="1">
-        <v>13.951388888888889</v>
+      <c r="L3" s="4">
+        <f t="shared" ref="L3:L35" si="0">H3*J3</f>
+        <v>1410</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="2">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1">
         <v>45757</v>
       </c>
       <c r="Q3" t="b">
@@ -1352,17 +1338,8 @@
       <c r="S3">
         <v>2001</v>
       </c>
-      <c r="T3" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3">
-        <v>777777777</v>
-      </c>
-      <c r="V3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>107001</v>
       </c>
@@ -1370,45 +1347,46 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H4">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1">
-        <v>3.8333333333333335</v>
+        <v>22</v>
+      </c>
+      <c r="J4" s="4">
+        <v>38</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="1">
-        <v>76.666666666666671</v>
+      <c r="L4" s="4">
+        <f t="shared" si="0"/>
+        <v>760</v>
       </c>
       <c r="M4" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="2">
+        <v>33</v>
+      </c>
+      <c r="P4" s="1">
         <v>45759</v>
       </c>
       <c r="Q4" t="b">
@@ -1420,17 +1398,8 @@
       <c r="S4">
         <v>2002</v>
       </c>
-      <c r="T4" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4">
-        <v>777777777</v>
-      </c>
-      <c r="V4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>107001</v>
       </c>
@@ -1438,45 +1407,46 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
         <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
       </c>
       <c r="H5">
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.28472222222222221</v>
+        <v>27</v>
+      </c>
+      <c r="J5" s="4">
+        <v>28</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="1">
-        <v>6.7847222222222223</v>
+      <c r="L5" s="4">
+        <f t="shared" si="0"/>
+        <v>700</v>
       </c>
       <c r="M5" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="2">
+        <v>33</v>
+      </c>
+      <c r="P5" s="1">
         <v>45759</v>
       </c>
       <c r="Q5" t="b">
@@ -1488,17 +1458,8 @@
       <c r="S5">
         <v>2002</v>
       </c>
-      <c r="T5" t="s">
-        <v>30</v>
-      </c>
-      <c r="U5">
-        <v>777777777</v>
-      </c>
-      <c r="V5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>107002</v>
       </c>
@@ -1506,45 +1467,46 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="H6">
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="1">
-        <v>3.25</v>
+        <v>22</v>
+      </c>
+      <c r="J6" s="4">
+        <v>32</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" s="1">
-        <v>26</v>
+      <c r="L6" s="4">
+        <f t="shared" si="0"/>
+        <v>256</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O6" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" s="2">
+        <v>40</v>
+      </c>
+      <c r="P6" s="1">
         <v>45762</v>
       </c>
       <c r="Q6" t="b">
@@ -1556,17 +1518,8 @@
       <c r="S6">
         <v>2003</v>
       </c>
-      <c r="T6" t="s">
-        <v>30</v>
-      </c>
-      <c r="U6">
-        <v>777777777</v>
-      </c>
-      <c r="V6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>107002</v>
       </c>
@@ -1574,45 +1527,46 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H7">
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.63888888888888884</v>
+        <v>42</v>
+      </c>
+      <c r="J7" s="4">
+        <v>64</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7" s="1">
-        <v>6.333333333333333</v>
+      <c r="L7" s="4">
+        <f t="shared" si="0"/>
+        <v>640</v>
       </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O7" t="s">
-        <v>53</v>
-      </c>
-      <c r="P7" s="2">
+        <v>40</v>
+      </c>
+      <c r="P7" s="1">
         <v>45762</v>
       </c>
       <c r="Q7" t="b">
@@ -1624,17 +1578,8 @@
       <c r="S7">
         <v>2003</v>
       </c>
-      <c r="T7" t="s">
-        <v>30</v>
-      </c>
-      <c r="U7">
-        <v>777777777</v>
-      </c>
-      <c r="V7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>107003</v>
       </c>
@@ -1642,45 +1587,46 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="1">
-        <v>2.7083333333333335</v>
+        <v>22</v>
+      </c>
+      <c r="J8" s="4">
+        <v>27</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="1">
-        <v>81.25</v>
+      <c r="L8" s="4">
+        <f t="shared" si="0"/>
+        <v>810</v>
       </c>
       <c r="M8" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" s="2">
+        <v>24</v>
+      </c>
+      <c r="P8" s="1">
         <v>45765</v>
       </c>
       <c r="Q8" t="b">
@@ -1692,17 +1638,8 @@
       <c r="S8">
         <v>2004</v>
       </c>
-      <c r="T8" t="s">
-        <v>30</v>
-      </c>
-      <c r="U8">
-        <v>777777777</v>
-      </c>
-      <c r="V8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>107003</v>
       </c>
@@ -1710,70 +1647,59 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9">
+        <v>70</v>
+      </c>
+      <c r="H9">
         <v>5</v>
       </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1.875</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>9.375</v>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="4">
+        <v>18</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="M9" t="s">
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O9" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" s="2">
+        <v>24</v>
+      </c>
+      <c r="P9" s="1">
         <v>45765</v>
       </c>
-      <c r="R9" t="b">
-        <v>0</v>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1004</v>
       </c>
       <c r="S9">
-        <v>1004</v>
-      </c>
-      <c r="T9">
         <v>2004</v>
       </c>
-      <c r="U9" t="s">
-        <v>30</v>
-      </c>
-      <c r="V9">
-        <v>777777777</v>
-      </c>
-      <c r="W9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>107003</v>
       </c>
@@ -1781,45 +1707,46 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="H10">
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.36805555555555558</v>
+        <v>27</v>
+      </c>
+      <c r="J10" s="4">
+        <v>37</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="1">
-        <v>3.5416666666666665</v>
+      <c r="L10" s="4">
+        <f t="shared" si="0"/>
+        <v>370</v>
       </c>
       <c r="M10" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O10" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" s="2">
+        <v>24</v>
+      </c>
+      <c r="P10" s="1">
         <v>45765</v>
       </c>
       <c r="Q10" t="b">
@@ -1831,17 +1758,8 @@
       <c r="S10">
         <v>2004</v>
       </c>
-      <c r="T10" t="s">
-        <v>30</v>
-      </c>
-      <c r="U10">
-        <v>777777777</v>
-      </c>
-      <c r="V10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>107004</v>
       </c>
@@ -1849,45 +1767,46 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="H11">
         <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="1">
-        <v>3.9583333333333335</v>
+        <v>22</v>
+      </c>
+      <c r="J11" s="4">
+        <v>39</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" s="1">
-        <v>98.958333333333329</v>
+      <c r="L11" s="4">
+        <f t="shared" si="0"/>
+        <v>975</v>
       </c>
       <c r="M11" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="2">
+        <v>33</v>
+      </c>
+      <c r="P11" s="1">
         <v>45767</v>
       </c>
       <c r="Q11" t="b">
@@ -1899,17 +1818,8 @@
       <c r="S11">
         <v>2005</v>
       </c>
-      <c r="T11" t="s">
-        <v>30</v>
-      </c>
-      <c r="U11">
-        <v>777777777</v>
-      </c>
-      <c r="V11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>107004</v>
       </c>
@@ -1917,45 +1827,46 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H12">
         <v>50</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0.18055555555555555</v>
+        <v>27</v>
+      </c>
+      <c r="J12" s="4">
+        <v>18</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12" s="1">
-        <v>8.75</v>
+      <c r="L12" s="4">
+        <f t="shared" si="0"/>
+        <v>900</v>
       </c>
       <c r="M12" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N12" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="2">
+        <v>33</v>
+      </c>
+      <c r="P12" s="1">
         <v>45767</v>
       </c>
       <c r="Q12" t="b">
@@ -1967,17 +1878,8 @@
       <c r="S12">
         <v>2005</v>
       </c>
-      <c r="T12" t="s">
-        <v>30</v>
-      </c>
-      <c r="U12">
-        <v>777777777</v>
-      </c>
-      <c r="V12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>107005</v>
       </c>
@@ -1985,45 +1887,46 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H13">
         <v>15</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="1">
-        <v>2.2916666666666665</v>
+        <v>22</v>
+      </c>
+      <c r="J13" s="4">
+        <v>22</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="1">
-        <v>34.375</v>
+      <c r="L13" s="4">
+        <f t="shared" si="0"/>
+        <v>330</v>
       </c>
       <c r="M13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O13" t="s">
-        <v>53</v>
-      </c>
-      <c r="P13" s="2">
+        <v>40</v>
+      </c>
+      <c r="P13" s="1">
         <v>45769</v>
       </c>
       <c r="Q13" t="b">
@@ -2035,17 +1938,8 @@
       <c r="S13">
         <v>2006</v>
       </c>
-      <c r="T13" t="s">
-        <v>30</v>
-      </c>
-      <c r="U13">
-        <v>777777777</v>
-      </c>
-      <c r="V13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>107005</v>
       </c>
@@ -2053,45 +1947,46 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H14">
         <v>20</v>
       </c>
       <c r="I14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0.29166666666666669</v>
+        <v>27</v>
+      </c>
+      <c r="J14" s="4">
+        <v>29</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" s="1">
-        <v>5.833333333333333</v>
+      <c r="L14" s="4">
+        <f t="shared" si="0"/>
+        <v>580</v>
       </c>
       <c r="M14" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N14" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O14" t="s">
-        <v>53</v>
-      </c>
-      <c r="P14" s="2">
+        <v>40</v>
+      </c>
+      <c r="P14" s="1">
         <v>45769</v>
       </c>
       <c r="Q14" t="b">
@@ -2103,17 +1998,8 @@
       <c r="S14">
         <v>2006</v>
       </c>
-      <c r="T14" t="s">
-        <v>30</v>
-      </c>
-      <c r="U14">
-        <v>777777777</v>
-      </c>
-      <c r="V14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>107006</v>
       </c>
@@ -2121,45 +2007,46 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="H15">
         <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="1">
-        <v>3.6666666666666665</v>
+        <v>22</v>
+      </c>
+      <c r="J15" s="4">
+        <v>36</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" s="1">
-        <v>44</v>
+      <c r="L15" s="4">
+        <f t="shared" si="0"/>
+        <v>432</v>
       </c>
       <c r="M15" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" s="2">
+        <v>24</v>
+      </c>
+      <c r="P15" s="1">
         <v>45772</v>
       </c>
       <c r="Q15" t="b">
@@ -2171,17 +2058,8 @@
       <c r="S15">
         <v>2007</v>
       </c>
-      <c r="T15" t="s">
-        <v>30</v>
-      </c>
-      <c r="U15">
-        <v>777777777</v>
-      </c>
-      <c r="V15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>107006</v>
       </c>
@@ -2189,70 +2067,59 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
-      </c>
-      <c r="H16" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16">
+        <v>71</v>
+      </c>
+      <c r="H16">
         <v>3</v>
       </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>7.5</v>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="4">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="M16" t="s">
+        <v>66</v>
       </c>
       <c r="N16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O16" t="s">
-        <v>28</v>
-      </c>
-      <c r="P16" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q16" s="2">
+        <v>24</v>
+      </c>
+      <c r="P16" s="1">
         <v>45772</v>
       </c>
-      <c r="R16" t="b">
-        <v>0</v>
+      <c r="Q16" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>1007</v>
       </c>
       <c r="S16">
-        <v>1007</v>
-      </c>
-      <c r="T16">
         <v>2007</v>
       </c>
-      <c r="U16" t="s">
-        <v>30</v>
-      </c>
-      <c r="V16">
-        <v>777777777</v>
-      </c>
-      <c r="W16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>107007</v>
       </c>
@@ -2260,45 +2127,46 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
         <v>59</v>
       </c>
-      <c r="F17" t="s">
-        <v>80</v>
-      </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="1">
-        <v>3.125</v>
+        <v>22</v>
+      </c>
+      <c r="J17" s="4">
+        <v>21</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" s="1">
-        <v>31.25</v>
+      <c r="L17" s="4">
+        <f t="shared" si="0"/>
+        <v>210</v>
       </c>
       <c r="M17" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N17" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O17" t="s">
-        <v>42</v>
-      </c>
-      <c r="P17" s="2">
+        <v>33</v>
+      </c>
+      <c r="P17" s="1">
         <v>45775</v>
       </c>
       <c r="Q17" t="b">
@@ -2310,17 +2178,8 @@
       <c r="S17">
         <v>2008</v>
       </c>
-      <c r="T17" t="s">
-        <v>30</v>
-      </c>
-      <c r="U17">
-        <v>777777777</v>
-      </c>
-      <c r="V17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>107007</v>
       </c>
@@ -2328,45 +2187,46 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H18">
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="1">
-        <v>3.9583333333333335</v>
+        <v>27</v>
+      </c>
+      <c r="J18" s="4">
+        <v>29</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18" s="1">
-        <v>15.833333333333334</v>
+      <c r="L18" s="4">
+        <f t="shared" si="0"/>
+        <v>116</v>
       </c>
       <c r="M18" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N18" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O18" t="s">
-        <v>42</v>
-      </c>
-      <c r="P18" s="2">
+        <v>33</v>
+      </c>
+      <c r="P18" s="1">
         <v>45775</v>
       </c>
       <c r="Q18" t="b">
@@ -2378,17 +2238,8 @@
       <c r="S18">
         <v>2008</v>
       </c>
-      <c r="T18" t="s">
-        <v>30</v>
-      </c>
-      <c r="U18">
-        <v>777777777</v>
-      </c>
-      <c r="V18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>107008</v>
       </c>
@@ -2396,45 +2247,46 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
         <v>21</v>
-      </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>25</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="1">
-        <v>3.5763888888888888</v>
+        <v>22</v>
+      </c>
+      <c r="J19" s="4">
+        <v>70</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19" s="1">
-        <v>35.625</v>
+      <c r="L19" s="4">
+        <f t="shared" si="0"/>
+        <v>700</v>
       </c>
       <c r="M19" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O19" t="s">
-        <v>29</v>
-      </c>
-      <c r="P19" s="2">
+        <v>24</v>
+      </c>
+      <c r="P19" s="1">
         <v>45818</v>
       </c>
       <c r="Q19" t="b">
@@ -2446,17 +2298,8 @@
       <c r="S19">
         <v>2009</v>
       </c>
-      <c r="T19" t="s">
-        <v>30</v>
-      </c>
-      <c r="U19">
-        <v>777777777</v>
-      </c>
-      <c r="V19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>107008</v>
       </c>
@@ -2464,45 +2307,46 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H20">
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.9375</v>
+        <v>27</v>
+      </c>
+      <c r="J20" s="4">
+        <v>94</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20" s="1">
-        <v>13.951388888888889</v>
+      <c r="L20" s="4">
+        <f t="shared" si="0"/>
+        <v>1410</v>
       </c>
       <c r="M20" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N20" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P20" s="2">
+        <v>24</v>
+      </c>
+      <c r="P20" s="1">
         <v>45818</v>
       </c>
       <c r="Q20" t="b">
@@ -2514,17 +2358,8 @@
       <c r="S20">
         <v>2009</v>
       </c>
-      <c r="T20" t="s">
-        <v>30</v>
-      </c>
-      <c r="U20">
-        <v>777777777</v>
-      </c>
-      <c r="V20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>107009</v>
       </c>
@@ -2532,45 +2367,46 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H21">
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="1">
-        <v>3.8333333333333335</v>
+        <v>22</v>
+      </c>
+      <c r="J21" s="4">
+        <v>38</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21" s="1">
-        <v>76.666666666666671</v>
+      <c r="L21" s="4">
+        <f t="shared" si="0"/>
+        <v>760</v>
       </c>
       <c r="M21" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N21" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O21" t="s">
-        <v>42</v>
-      </c>
-      <c r="P21" s="2">
+        <v>33</v>
+      </c>
+      <c r="P21" s="1">
         <v>45820</v>
       </c>
       <c r="Q21" t="b">
@@ -2582,17 +2418,8 @@
       <c r="S21">
         <v>2010</v>
       </c>
-      <c r="T21" t="s">
-        <v>30</v>
-      </c>
-      <c r="U21">
-        <v>777777777</v>
-      </c>
-      <c r="V21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>107009</v>
       </c>
@@ -2600,45 +2427,46 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
         <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
       </c>
       <c r="H22">
         <v>25</v>
       </c>
       <c r="I22" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0.28472222222222221</v>
+        <v>27</v>
+      </c>
+      <c r="J22" s="4">
+        <v>28</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22" s="1">
-        <v>6.7847222222222223</v>
+      <c r="L22" s="4">
+        <f t="shared" si="0"/>
+        <v>700</v>
       </c>
       <c r="M22" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N22" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O22" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22" s="2">
+        <v>33</v>
+      </c>
+      <c r="P22" s="1">
         <v>45820</v>
       </c>
       <c r="Q22" t="b">
@@ -2650,17 +2478,8 @@
       <c r="S22">
         <v>2010</v>
       </c>
-      <c r="T22" t="s">
-        <v>30</v>
-      </c>
-      <c r="U22">
-        <v>777777777</v>
-      </c>
-      <c r="V22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>107010</v>
       </c>
@@ -2668,45 +2487,46 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F23" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="H23">
         <v>8</v>
       </c>
       <c r="I23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="1">
-        <v>3.25</v>
+        <v>22</v>
+      </c>
+      <c r="J23" s="4">
+        <v>32</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23" s="1">
-        <v>26</v>
+      <c r="L23" s="4">
+        <f t="shared" si="0"/>
+        <v>256</v>
       </c>
       <c r="M23" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N23" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O23" t="s">
-        <v>53</v>
-      </c>
-      <c r="P23" s="2">
+        <v>40</v>
+      </c>
+      <c r="P23" s="1">
         <v>45823</v>
       </c>
       <c r="Q23" t="b">
@@ -2718,17 +2538,8 @@
       <c r="S23">
         <v>2011</v>
       </c>
-      <c r="T23" t="s">
-        <v>30</v>
-      </c>
-      <c r="U23">
-        <v>777777777</v>
-      </c>
-      <c r="V23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>107010</v>
       </c>
@@ -2736,45 +2547,46 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>56</v>
-      </c>
-      <c r="J24" s="3">
-        <v>0.63888888888888884</v>
+        <v>42</v>
+      </c>
+      <c r="J24" s="4">
+        <v>64</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
-      <c r="L24" s="1">
-        <v>6.333333333333333</v>
+      <c r="L24" s="4">
+        <f t="shared" si="0"/>
+        <v>640</v>
       </c>
       <c r="M24" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N24" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O24" t="s">
-        <v>53</v>
-      </c>
-      <c r="P24" s="2">
+        <v>40</v>
+      </c>
+      <c r="P24" s="1">
         <v>45823</v>
       </c>
       <c r="Q24" t="b">
@@ -2786,17 +2598,8 @@
       <c r="S24">
         <v>2011</v>
       </c>
-      <c r="T24" t="s">
-        <v>30</v>
-      </c>
-      <c r="U24">
-        <v>777777777</v>
-      </c>
-      <c r="V24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>107011</v>
       </c>
@@ -2804,45 +2607,46 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="H25">
         <v>30</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J25" s="1">
-        <v>2.7083333333333335</v>
+        <v>22</v>
+      </c>
+      <c r="J25" s="4">
+        <v>27</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
-      <c r="L25" s="1">
-        <v>81.25</v>
+      <c r="L25" s="4">
+        <f t="shared" si="0"/>
+        <v>810</v>
       </c>
       <c r="M25" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O25" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" s="2">
+        <v>24</v>
+      </c>
+      <c r="P25" s="1">
         <v>45826</v>
       </c>
       <c r="Q25" t="b">
@@ -2854,17 +2658,8 @@
       <c r="S25">
         <v>2012</v>
       </c>
-      <c r="T25" t="s">
-        <v>30</v>
-      </c>
-      <c r="U25">
-        <v>777777777</v>
-      </c>
-      <c r="V25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>107011</v>
       </c>
@@ -2872,70 +2667,59 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" t="s">
-        <v>64</v>
-      </c>
-      <c r="I26">
+        <v>70</v>
+      </c>
+      <c r="H26">
         <v>5</v>
       </c>
-      <c r="J26" t="s">
-        <v>34</v>
-      </c>
-      <c r="K26" s="1">
-        <v>1.875</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26" s="1">
-        <v>9.375</v>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="4">
+        <v>19</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="M26" t="s">
+        <v>66</v>
       </c>
       <c r="N26" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O26" t="s">
-        <v>28</v>
-      </c>
-      <c r="P26" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q26" s="2">
+        <v>24</v>
+      </c>
+      <c r="P26" s="1">
         <v>45826</v>
       </c>
-      <c r="R26" t="b">
-        <v>0</v>
+      <c r="Q26" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>1012</v>
       </c>
       <c r="S26">
-        <v>1012</v>
-      </c>
-      <c r="T26">
         <v>2012</v>
       </c>
-      <c r="U26" t="s">
-        <v>30</v>
-      </c>
-      <c r="V26">
-        <v>777777777</v>
-      </c>
-      <c r="W26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>107011</v>
       </c>
@@ -2943,45 +2727,46 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="H27">
         <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="3">
-        <v>0.36805555555555558</v>
+        <v>27</v>
+      </c>
+      <c r="J27" s="4">
+        <v>39</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27" s="1">
-        <v>3.5416666666666665</v>
+      <c r="L27" s="4">
+        <f t="shared" si="0"/>
+        <v>390</v>
       </c>
       <c r="M27" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N27" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O27" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27" s="2">
+        <v>24</v>
+      </c>
+      <c r="P27" s="1">
         <v>45826</v>
       </c>
       <c r="Q27" t="b">
@@ -2993,17 +2778,8 @@
       <c r="S27">
         <v>2012</v>
       </c>
-      <c r="T27" t="s">
-        <v>30</v>
-      </c>
-      <c r="U27">
-        <v>777777777</v>
-      </c>
-      <c r="V27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>107012</v>
       </c>
@@ -3011,45 +2787,46 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G28" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="H28">
         <v>25</v>
       </c>
       <c r="I28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J28" s="1">
-        <v>3.9583333333333335</v>
+        <v>22</v>
+      </c>
+      <c r="J28" s="4">
+        <v>39</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28" s="1">
-        <v>98.958333333333329</v>
+      <c r="L28" s="4">
+        <f t="shared" si="0"/>
+        <v>975</v>
       </c>
       <c r="M28" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N28" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O28" t="s">
-        <v>42</v>
-      </c>
-      <c r="P28" s="2">
+        <v>33</v>
+      </c>
+      <c r="P28" s="1">
         <v>45828</v>
       </c>
       <c r="Q28" t="b">
@@ -3061,17 +2838,8 @@
       <c r="S28">
         <v>2013</v>
       </c>
-      <c r="T28" t="s">
-        <v>30</v>
-      </c>
-      <c r="U28">
-        <v>777777777</v>
-      </c>
-      <c r="V28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>107012</v>
       </c>
@@ -3079,45 +2847,46 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G29" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H29">
         <v>50</v>
       </c>
       <c r="I29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J29" s="3">
-        <v>0.18055555555555555</v>
+        <v>27</v>
+      </c>
+      <c r="J29" s="4">
+        <v>18</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29" s="1">
-        <v>8.75</v>
+      <c r="L29" s="4">
+        <f t="shared" si="0"/>
+        <v>900</v>
       </c>
       <c r="M29" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N29" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O29" t="s">
-        <v>42</v>
-      </c>
-      <c r="P29" s="2">
+        <v>33</v>
+      </c>
+      <c r="P29" s="1">
         <v>45828</v>
       </c>
       <c r="Q29" t="b">
@@ -3129,17 +2898,8 @@
       <c r="S29">
         <v>2013</v>
       </c>
-      <c r="T29" t="s">
-        <v>30</v>
-      </c>
-      <c r="U29">
-        <v>777777777</v>
-      </c>
-      <c r="V29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>107013</v>
       </c>
@@ -3147,45 +2907,46 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H30">
         <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" s="1">
-        <v>2.2916666666666665</v>
+        <v>22</v>
+      </c>
+      <c r="J30" s="4">
+        <v>29</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
-      <c r="L30" s="1">
-        <v>34.375</v>
+      <c r="L30" s="4">
+        <f t="shared" si="0"/>
+        <v>435</v>
       </c>
       <c r="M30" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N30" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O30" t="s">
-        <v>53</v>
-      </c>
-      <c r="P30" s="2">
+        <v>40</v>
+      </c>
+      <c r="P30" s="1">
         <v>45830</v>
       </c>
       <c r="Q30" t="b">
@@ -3197,17 +2958,8 @@
       <c r="S30">
         <v>2014</v>
       </c>
-      <c r="T30" t="s">
-        <v>30</v>
-      </c>
-      <c r="U30">
-        <v>777777777</v>
-      </c>
-      <c r="V30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>107013</v>
       </c>
@@ -3215,45 +2967,46 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H31">
         <v>20</v>
       </c>
       <c r="I31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="3">
-        <v>0.29166666666666669</v>
+        <v>27</v>
+      </c>
+      <c r="J31" s="4">
+        <v>29</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
-      <c r="L31" s="1">
-        <v>5.833333333333333</v>
+      <c r="L31" s="4">
+        <f t="shared" si="0"/>
+        <v>580</v>
       </c>
       <c r="M31" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="O31" t="s">
-        <v>53</v>
-      </c>
-      <c r="P31" s="2">
+        <v>40</v>
+      </c>
+      <c r="P31" s="1">
         <v>45830</v>
       </c>
       <c r="Q31" t="b">
@@ -3265,17 +3018,8 @@
       <c r="S31">
         <v>2014</v>
       </c>
-      <c r="T31" t="s">
-        <v>30</v>
-      </c>
-      <c r="U31">
-        <v>777777777</v>
-      </c>
-      <c r="V31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>107014</v>
       </c>
@@ -3283,45 +3027,46 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E32" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="H32">
         <v>12</v>
       </c>
       <c r="I32" t="s">
-        <v>26</v>
-      </c>
-      <c r="J32" s="1">
-        <v>3.6666666666666665</v>
+        <v>22</v>
+      </c>
+      <c r="J32" s="4">
+        <v>36</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
-      <c r="L32" s="1">
-        <v>44</v>
+      <c r="L32" s="4">
+        <f t="shared" si="0"/>
+        <v>432</v>
       </c>
       <c r="M32" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="N32" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O32" t="s">
-        <v>29</v>
-      </c>
-      <c r="P32" s="2">
+        <v>24</v>
+      </c>
+      <c r="P32" s="1">
         <v>45833</v>
       </c>
       <c r="Q32" t="b">
@@ -3333,17 +3078,8 @@
       <c r="S32">
         <v>2015</v>
       </c>
-      <c r="T32" t="s">
-        <v>30</v>
-      </c>
-      <c r="U32">
-        <v>777777777</v>
-      </c>
-      <c r="V32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>107014</v>
       </c>
@@ -3351,70 +3087,59 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="G33" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" t="s">
-        <v>79</v>
-      </c>
-      <c r="I33">
+        <v>71</v>
+      </c>
+      <c r="H33">
         <v>3</v>
       </c>
-      <c r="J33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33" s="1">
-        <v>7.5</v>
+      <c r="I33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" s="4">
+        <v>25</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="M33" t="s">
+        <v>66</v>
       </c>
       <c r="N33" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O33" t="s">
-        <v>28</v>
-      </c>
-      <c r="P33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q33" s="2">
+        <v>24</v>
+      </c>
+      <c r="P33" s="1">
         <v>45833</v>
       </c>
-      <c r="R33" t="b">
-        <v>0</v>
+      <c r="Q33" t="b">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>1015</v>
       </c>
       <c r="S33">
-        <v>1015</v>
-      </c>
-      <c r="T33">
         <v>2015</v>
       </c>
-      <c r="U33" t="s">
-        <v>30</v>
-      </c>
-      <c r="V33">
-        <v>777777777</v>
-      </c>
-      <c r="W33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>107015</v>
       </c>
@@ -3422,45 +3147,46 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
         <v>59</v>
       </c>
-      <c r="F34" t="s">
-        <v>80</v>
-      </c>
       <c r="G34" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="H34">
         <v>10</v>
       </c>
       <c r="I34" t="s">
-        <v>26</v>
-      </c>
-      <c r="J34" s="1">
-        <v>3.125</v>
+        <v>22</v>
+      </c>
+      <c r="J34" s="4">
+        <v>31</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
-      <c r="L34" s="1">
-        <v>31.25</v>
+      <c r="L34" s="4">
+        <f t="shared" si="0"/>
+        <v>310</v>
       </c>
       <c r="M34" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N34" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O34" t="s">
-        <v>42</v>
-      </c>
-      <c r="P34" s="2">
+        <v>33</v>
+      </c>
+      <c r="P34" s="1">
         <v>45836</v>
       </c>
       <c r="Q34" t="b">
@@ -3472,17 +3198,8 @@
       <c r="S34">
         <v>2016</v>
       </c>
-      <c r="T34" t="s">
-        <v>30</v>
-      </c>
-      <c r="U34">
-        <v>777777777</v>
-      </c>
-      <c r="V34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>107015</v>
       </c>
@@ -3490,45 +3207,46 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F35" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="H35">
         <v>4</v>
       </c>
       <c r="I35" t="s">
-        <v>34</v>
-      </c>
-      <c r="J35" s="1">
-        <v>3.9583333333333335</v>
+        <v>27</v>
+      </c>
+      <c r="J35" s="4">
+        <v>29</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
-      <c r="L35" s="1">
-        <v>15.833333333333334</v>
+      <c r="L35" s="4">
+        <f t="shared" si="0"/>
+        <v>116</v>
       </c>
       <c r="M35" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N35" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="O35" t="s">
-        <v>42</v>
-      </c>
-      <c r="P35" s="2">
+        <v>33</v>
+      </c>
+      <c r="P35" s="1">
         <v>45836</v>
       </c>
       <c r="Q35" t="b">
@@ -3540,14 +3258,107 @@
       <c r="S35">
         <v>2016</v>
       </c>
-      <c r="T35" t="s">
-        <v>30</v>
-      </c>
-      <c r="U35">
-        <v>777777777</v>
-      </c>
-      <c r="V35" t="s">
-        <v>43</v>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>107021</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" s="4">
+        <v>400</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36" s="4">
+        <f t="shared" ref="L36" si="1">H36*J36</f>
+        <v>1200</v>
+      </c>
+      <c r="M36" t="s">
+        <v>66</v>
+      </c>
+      <c r="N36" t="s">
+        <v>23</v>
+      </c>
+      <c r="O36" t="s">
+        <v>24</v>
+      </c>
+      <c r="P36" s="1">
+        <v>45833</v>
+      </c>
+      <c r="Q36" t="b">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>1015</v>
+      </c>
+      <c r="S36">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>107021</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37">
+        <v>10</v>
+      </c>
+      <c r="I37" t="s">
+        <v>27</v>
+      </c>
+      <c r="J37" s="4">
+        <v>79</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4">
+        <f t="shared" ref="L37" si="2">H37*J37</f>
+        <v>790</v>
+      </c>
+      <c r="M37" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>